<commit_message>
update for data in 2021-12: single-file sestava from MMR
</commit_message>
<xml_diff>
--- a/data-manual/prj_nehierarchicke-vybrano.xlsx
+++ b/data-manual/prj_nehierarchicke-vybrano.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11202"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petr/cwork/mmr-esif-clean/data-manual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petr/cwork/mmr-esif-clean-202112/data-manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF73BB48-BBF2-D649-88BD-9042DAE343B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBE14AE-2195-2042-8273-D926EA51CFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32560" yWindow="-6680" windowWidth="39560" windowHeight="24900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9572" uniqueCount="2008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9638" uniqueCount="2008">
   <si>
     <t>op_id</t>
   </si>
@@ -6435,15 +6435,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P742"/>
+  <dimension ref="A1:P747"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B715" workbookViewId="0">
+      <selection activeCell="F746" sqref="F746"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="63.6640625" customWidth="1"/>
+    <col min="10" max="10" width="32" customWidth="1"/>
     <col min="15" max="15" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -24075,7 +24076,7 @@
         <v>50</v>
       </c>
       <c r="F384" t="s">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="H384" t="s">
         <v>1097</v>
@@ -40620,6 +40621,238 @@
       </c>
       <c r="P742" t="s">
         <v>2003</v>
+      </c>
+    </row>
+    <row r="743" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A743" t="s">
+        <v>16</v>
+      </c>
+      <c r="B743" t="s">
+        <v>17</v>
+      </c>
+      <c r="C743" t="s">
+        <v>18</v>
+      </c>
+      <c r="D743" t="s">
+        <v>19</v>
+      </c>
+      <c r="E743" t="s">
+        <v>20</v>
+      </c>
+      <c r="F743" t="s">
+        <v>2006</v>
+      </c>
+      <c r="H743" t="s">
+        <v>21</v>
+      </c>
+      <c r="I743" t="b">
+        <v>0</v>
+      </c>
+      <c r="J743" t="s">
+        <v>22</v>
+      </c>
+      <c r="K743" t="s">
+        <v>23</v>
+      </c>
+      <c r="M743" t="s">
+        <v>24</v>
+      </c>
+      <c r="N743" t="s">
+        <v>25</v>
+      </c>
+      <c r="O743" t="s">
+        <v>23</v>
+      </c>
+      <c r="P743" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="744" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A744" t="s">
+        <v>16</v>
+      </c>
+      <c r="B744" t="s">
+        <v>17</v>
+      </c>
+      <c r="C744" t="s">
+        <v>26</v>
+      </c>
+      <c r="D744" t="s">
+        <v>27</v>
+      </c>
+      <c r="E744" t="s">
+        <v>28</v>
+      </c>
+      <c r="F744" t="s">
+        <v>2005</v>
+      </c>
+      <c r="H744" t="s">
+        <v>21</v>
+      </c>
+      <c r="I744" t="b">
+        <v>0</v>
+      </c>
+      <c r="J744" t="s">
+        <v>22</v>
+      </c>
+      <c r="K744" t="s">
+        <v>29</v>
+      </c>
+      <c r="L744" t="b">
+        <v>0</v>
+      </c>
+      <c r="M744" t="s">
+        <v>24</v>
+      </c>
+      <c r="N744" t="s">
+        <v>25</v>
+      </c>
+      <c r="O744" t="s">
+        <v>23</v>
+      </c>
+      <c r="P744" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="745" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A745" t="s">
+        <v>16</v>
+      </c>
+      <c r="B745" t="s">
+        <v>17</v>
+      </c>
+      <c r="C745" t="s">
+        <v>30</v>
+      </c>
+      <c r="D745" t="s">
+        <v>31</v>
+      </c>
+      <c r="E745" t="s">
+        <v>28</v>
+      </c>
+      <c r="F745" t="s">
+        <v>2005</v>
+      </c>
+      <c r="G745" t="s">
+        <v>32</v>
+      </c>
+      <c r="H745" t="s">
+        <v>21</v>
+      </c>
+      <c r="I745" t="b">
+        <v>0</v>
+      </c>
+      <c r="J745" t="s">
+        <v>22</v>
+      </c>
+      <c r="K745" t="s">
+        <v>33</v>
+      </c>
+      <c r="L745" t="b">
+        <v>0</v>
+      </c>
+      <c r="M745" t="s">
+        <v>24</v>
+      </c>
+      <c r="N745" t="s">
+        <v>25</v>
+      </c>
+      <c r="O745" t="s">
+        <v>23</v>
+      </c>
+      <c r="P745" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="746" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A746" t="s">
+        <v>16</v>
+      </c>
+      <c r="B746" t="s">
+        <v>34</v>
+      </c>
+      <c r="C746" t="s">
+        <v>35</v>
+      </c>
+      <c r="D746" t="s">
+        <v>36</v>
+      </c>
+      <c r="E746" t="s">
+        <v>37</v>
+      </c>
+      <c r="F746" t="s">
+        <v>2006</v>
+      </c>
+      <c r="H746" t="s">
+        <v>38</v>
+      </c>
+      <c r="I746" t="b">
+        <v>0</v>
+      </c>
+      <c r="J746" t="s">
+        <v>39</v>
+      </c>
+      <c r="M746" t="s">
+        <v>40</v>
+      </c>
+      <c r="N746" t="s">
+        <v>41</v>
+      </c>
+      <c r="O746" t="s">
+        <v>42</v>
+      </c>
+      <c r="P746" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="747" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A747" t="s">
+        <v>16</v>
+      </c>
+      <c r="B747" t="s">
+        <v>34</v>
+      </c>
+      <c r="C747" t="s">
+        <v>44</v>
+      </c>
+      <c r="D747" t="s">
+        <v>45</v>
+      </c>
+      <c r="E747" t="s">
+        <v>20</v>
+      </c>
+      <c r="F747" t="s">
+        <v>2005</v>
+      </c>
+      <c r="G747" t="s">
+        <v>32</v>
+      </c>
+      <c r="H747" t="s">
+        <v>38</v>
+      </c>
+      <c r="I747" t="b">
+        <v>0</v>
+      </c>
+      <c r="J747" t="s">
+        <v>39</v>
+      </c>
+      <c r="K747" t="s">
+        <v>46</v>
+      </c>
+      <c r="L747" t="b">
+        <v>0</v>
+      </c>
+      <c r="M747" t="s">
+        <v>40</v>
+      </c>
+      <c r="N747" t="s">
+        <v>41</v>
+      </c>
+      <c r="O747" t="s">
+        <v>42</v>
+      </c>
+      <c r="P747" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>